<commit_message>
Completed implementation of Dijkstra's algorithm and applied it to build routing tables
</commit_message>
<xml_diff>
--- a/Assignment2/DevLog.xlsx
+++ b/Assignment2/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7E35BB-9394-4FCE-AE2C-3A6D444A80D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F7FD1-09C9-41B2-B8BD-547E32EC232F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="1635" yWindow="1275" windowWidth="22980" windowHeight="18030" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Bronson Billing (575952)</t>
-  </si>
-  <si>
-    <t>Database implementation where two data structures are compared with each other for performance. This particular project involves a database of UFC fighters and event codes.</t>
   </si>
   <si>
     <t>https://github.com/BronsonKBilling/KIT205_575952</t>
@@ -117,6 +114,27 @@
   </si>
   <si>
     <t>KIT205 Assignment 2 - Graph</t>
+  </si>
+  <si>
+    <t>Routing protocol demonstration comparing how quickly two shortest path algorithms (Dijkstra's and Bellman-Ford) reach convergence in a simulated network. This compares the algorithms used in two routing protocols, the now dated RIP (Bellman-Ford) and the dominant OSPF (Dijkstra).</t>
+  </si>
+  <si>
+    <t>Not a milestone - Completed implementation of Dijkstra's algorithm and its associated helper functions. Completed implementation of main routing table builder function</t>
+  </si>
+  <si>
+    <t>build_routing_tables
+find_shortest_paths_dijkstra
+all_devices_known</t>
+  </si>
+  <si>
+    <t>test_graph - The functions that were implemented in this commit have not yet been tested. The point at which they are tested will mark a milestone</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to check whether my implementation of Dijkstra's algorithm was correct or not. It discovered two minor errors that it helped to fix.
+Notes taken from the weekly content that focused on Dijkstra's algorithm were used for building the implementation of th algorithm</t>
+  </si>
+  <si>
+    <t>I also added a file that contains the full routing table for all 'devices' in the test_graph file. This commit made use of my notes on the weekly content, then my implementation based on that content was assessed by ChatGPT for accuracy.</t>
   </si>
 </sst>
 </file>
@@ -212,7 +230,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -255,14 +273,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -620,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +658,7 @@
     <col min="7" max="7" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -645,33 +666,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -679,11 +700,11 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
@@ -703,57 +724,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12">
+        <v>45809</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="17">
+        <v>45801</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="18">
-        <v>45801</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="E10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45797</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12">
-        <v>45797</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="10"/>
       <c r="C12" s="12"/>
@@ -762,7 +796,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="10"/>
       <c r="C13" s="12"/>
@@ -771,7 +805,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="10"/>
       <c r="C14" s="12"/>
@@ -780,8 +814,8 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
       <c r="B15" s="10"/>
       <c r="C15" s="12"/>
       <c r="D15" s="10"/>
@@ -789,25 +823,25 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="12"/>
       <c r="D18" s="10"/>
@@ -815,7 +849,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="12"/>
@@ -824,7 +858,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="10"/>
       <c r="C20" s="12"/>
@@ -833,33 +867,33 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+    <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2"/>
@@ -868,8 +902,9 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1172,12 +1207,20 @@
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
MILESTONE: tests for dijkstra's algorithm function have been completed. This means that the first algorithm to be compared has been fully implemented.
</commit_message>
<xml_diff>
--- a/Assignment2/DevLog.xlsx
+++ b/Assignment2/DevLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F7FD1-09C9-41B2-B8BD-547E32EC232F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDAECF2-8C19-4E18-A788-3B4CF896F4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="1275" windowWidth="22980" windowHeight="18030" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -135,6 +135,24 @@
   </si>
   <si>
     <t>I also added a file that contains the full routing table for all 'devices' in the test_graph file. This commit made use of my notes on the weekly content, then my implementation based on that content was assessed by ChatGPT for accuracy.</t>
+  </si>
+  <si>
+    <t>Milestone - Dijkstra's algorithm function for building a routing table has been completed as the testing function has now implemented tests for it. The tests go through every execution path and realistic case for a computer network</t>
+  </si>
+  <si>
+    <t>test_network
+find_shortest_paths_dijkstra
+add_link
+all_devices_known</t>
+  </si>
+  <si>
+    <t>ChatGPT was used minimally for debugging, and it was used to come up with ideas for test cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_graph - Executes every possible execution path of all functions in the network.c file. It tests all likely and allowed network configurations that could be fed into find_shortest_paths_dijkstra. </t>
+  </si>
+  <si>
+    <t>In addition to completing the testing function, I needed to make fixes to other functions and needed to correct some oversights made in prior commits.</t>
   </si>
 </sst>
 </file>
@@ -641,9 +659,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -724,77 +742,89 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12">
+        <v>45811</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="12">
         <v>45809</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C11" s="17">
         <v>45801</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C12" s="12">
         <v>45797</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -814,7 +844,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="10"/>
       <c r="C15" s="12"/>
@@ -823,8 +853,8 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
       <c r="B16" s="10"/>
       <c r="C16" s="12"/>
       <c r="D16" s="10"/>
@@ -832,25 +862,25 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="12"/>
       <c r="D19" s="10"/>
@@ -858,7 +888,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="10"/>
       <c r="C20" s="12"/>
@@ -867,7 +897,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="10"/>
       <c r="C21" s="12"/>
@@ -876,33 +906,33 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+    <row r="22" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
@@ -911,8 +941,9 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1215,12 +1246,20 @@
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Completed implementation of Bellman-Ford algorithm and applied it to building routing tables.
</commit_message>
<xml_diff>
--- a/Assignment2/DevLog.xlsx
+++ b/Assignment2/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDAECF2-8C19-4E18-A788-3B4CF896F4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553DDA7-F656-406E-A040-18F0499E80AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="1275" windowWidth="22980" windowHeight="18030" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -153,6 +153,22 @@
   </si>
   <si>
     <t>In addition to completing the testing function, I needed to make fixes to other functions and needed to correct some oversights made in prior commits.</t>
+  </si>
+  <si>
+    <t>Not a milestone - Completed implementation of Bellman-Ford algorithm and separated the routing table building part of both the dijkstra function and the Bellman-Ford function to a separate helper function</t>
+  </si>
+  <si>
+    <t>find_shortest_paths_bellman_ford
+build_routing_table_from_distances</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to make pseudocode that helped me to learn about the Bellman-Ford algorithm, also helped with basic debugging</t>
+  </si>
+  <si>
+    <t>test_graph - This function does not fully test the Bellman-Ford function yet, it just does a basic adhoc test to see if the function actually works</t>
+  </si>
+  <si>
+    <t>The code for both the Dijkstra and Bellman-Ford algorithm could use further refactoring to avoid code duplication. The easiest of which has already been done, which was moving the routing table building to build_routing_table_from_distances</t>
   </si>
 </sst>
 </file>
@@ -659,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -742,98 +758,110 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C9" s="12">
         <v>45811</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45811</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C11" s="12">
         <v>45809</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C12" s="17">
         <v>45801</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="10" t="s">
+    <row r="13" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="12">
         <v>45797</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -853,7 +881,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="10"/>
       <c r="C16" s="12"/>
@@ -862,8 +890,8 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
       <c r="B17" s="10"/>
       <c r="C17" s="12"/>
       <c r="D17" s="10"/>
@@ -871,25 +899,25 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="12"/>
       <c r="D20" s="10"/>
@@ -897,7 +925,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="10"/>
       <c r="C21" s="12"/>
@@ -906,7 +934,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="10"/>
       <c r="C22" s="12"/>
@@ -915,33 +943,33 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+    <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
@@ -950,8 +978,9 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1254,12 +1283,20 @@
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
MILESTONE: Completed implementation of tests for Bellman-Ford function, added helper functions to make printing test values easier
</commit_message>
<xml_diff>
--- a/Assignment2/DevLog.xlsx
+++ b/Assignment2/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553DDA7-F656-406E-A040-18F0499E80AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88E0FC4-904B-4452-A93A-D65A58CA16FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="1275" windowWidth="22980" windowHeight="18030" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -127,9 +127,6 @@
 all_devices_known</t>
   </si>
   <si>
-    <t>test_graph - The functions that were implemented in this commit have not yet been tested. The point at which they are tested will mark a milestone</t>
-  </si>
-  <si>
     <t>ChatGPT was used to check whether my implementation of Dijkstra's algorithm was correct or not. It discovered two minor errors that it helped to fix.
 Notes taken from the weekly content that focused on Dijkstra's algorithm were used for building the implementation of th algorithm</t>
   </si>
@@ -149,9 +146,6 @@
     <t>ChatGPT was used minimally for debugging, and it was used to come up with ideas for test cases.</t>
   </si>
   <si>
-    <t xml:space="preserve">test_graph - Executes every possible execution path of all functions in the network.c file. It tests all likely and allowed network configurations that could be fed into find_shortest_paths_dijkstra. </t>
-  </si>
-  <si>
     <t>In addition to completing the testing function, I needed to make fixes to other functions and needed to correct some oversights made in prior commits.</t>
   </si>
   <si>
@@ -165,10 +159,34 @@
     <t>ChatGPT was used to make pseudocode that helped me to learn about the Bellman-Ford algorithm, also helped with basic debugging</t>
   </si>
   <si>
-    <t>test_graph - This function does not fully test the Bellman-Ford function yet, it just does a basic adhoc test to see if the function actually works</t>
-  </si>
-  <si>
     <t>The code for both the Dijkstra and Bellman-Ford algorithm could use further refactoring to avoid code duplication. The easiest of which has already been done, which was moving the routing table building to build_routing_table_from_distances</t>
+  </si>
+  <si>
+    <t>Milestone - Finished implementing tests for the Bellman-Ford algorithm function. It has been thoroughly tested along all execution paths and potential network conditions. This means that both algorithms have been implemented and comparisons can begin</t>
+  </si>
+  <si>
+    <t>find_shortest_paths_bellman_ford
+print_routes
+print_routes_from_test_file
+test_network</t>
+  </si>
+  <si>
+    <t>ChatGPT was used for troubleshooting code issues</t>
+  </si>
+  <si>
+    <t>test_network - This function does not fully test the Bellman-Ford function yet, it just does a basic adhoc test to see if the function actually works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_network - Executes every possible execution path of all functions in the network.c file. It tests all likely and allowed network configurations that could be fed into find_shortest_paths_dijkstra. </t>
+  </si>
+  <si>
+    <t>test_network - The functions that were implemented in this commit have not yet been tested. The point at which they are tested will mark a milestone</t>
+  </si>
+  <si>
+    <t>test_network - The function now tests The Bellman-Ford algorithm function and sees if it can accurately build routing tables for different network conditions. All execution paths are reached by the tests. Extra tests were also added for build_routing_table_from_distances, which was added in the previous commit</t>
+  </si>
+  <si>
+    <t>Tests were heavily refactored in this commit. The tests (especially printing expected and actual routes) had code duplication between them, so helper printing functions were added to remedy this.</t>
   </si>
 </sst>
 </file>
@@ -675,9 +693,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -731,7 +749,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9">
-        <v>45760</v>
+        <v>45797</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.4">
@@ -758,119 +776,131 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="12">
-        <v>45811</v>
+        <v>45812</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" s="12">
         <v>45811</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45811</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C12" s="12">
         <v>45809</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C13" s="17">
         <v>45801</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G13" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="10" t="s">
+    <row r="14" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="12">
         <v>45797</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -890,7 +920,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="10"/>
       <c r="C17" s="12"/>
@@ -899,8 +929,8 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
       <c r="B18" s="10"/>
       <c r="C18" s="12"/>
       <c r="D18" s="10"/>
@@ -908,25 +938,25 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="12"/>
       <c r="D21" s="10"/>
@@ -934,7 +964,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="10"/>
       <c r="C22" s="12"/>
@@ -943,7 +973,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="10"/>
       <c r="C23" s="12"/>
@@ -952,33 +982,33 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+    <row r="24" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
@@ -987,8 +1017,9 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1291,12 +1322,20 @@
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
MILESTONE: Completed algorithm comparison function and added network deletion function. All necessary code for the assignment 2 has now been completed with this commit. Also generated test files
</commit_message>
<xml_diff>
--- a/Assignment2/DevLog.xlsx
+++ b/Assignment2/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88E0FC4-904B-4452-A93A-D65A58CA16FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB7BF36-3CFC-4E97-81F9-063668B0E5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -187,6 +187,23 @@
   </si>
   <si>
     <t>Tests were heavily refactored in this commit. The tests (especially printing expected and actual routes) had code duplication between them, so helper printing functions were added to remedy this.</t>
+  </si>
+  <si>
+    <t>delete_network
+test_network
+compare_algorithms</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to generate python code that was used to generate network files for algorithm comparison.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_network - This function was changed slightly to free dynamically allocated memory at the end of its execution. This is needed as the comparison function runs right after it.  </t>
+  </si>
+  <si>
+    <t>Milestone - Finished implementing algorithm comparison function. Both algorithms are compared to eachother to see how quickly they can build a full routing table for each device on the network. Also added helper function to delete network and free memory. This marks the point where all code for the assignment has been completed.</t>
+  </si>
+  <si>
+    <t>I also cleaned up quite a bit of the code and added comments to functions that needed them. I had far less commits with this assignment compared to the last one, I believe a large reason for this was due to my development practices getting better. There were far fewer mistakes that needed correcting with this function, and I made sure that functions were maintainable and readable as I was writing them, rather than last time when I needed to make multiple correction commits.</t>
   </si>
 </sst>
 </file>
@@ -693,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,140 +793,152 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C9" s="12">
-        <v>45812</v>
+        <v>45813</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10" s="12">
-        <v>45811</v>
+        <v>45812</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" s="12">
         <v>45811</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="12">
+        <v>45811</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="12">
         <v>45809</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C14" s="17">
         <v>45801</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G14" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10" t="s">
+    <row r="15" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C15" s="12">
         <v>45797</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -929,7 +958,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="10"/>
       <c r="C18" s="12"/>
@@ -938,8 +967,8 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
       <c r="B19" s="10"/>
       <c r="C19" s="12"/>
       <c r="D19" s="10"/>
@@ -947,25 +976,25 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="12"/>
       <c r="D22" s="10"/>
@@ -973,7 +1002,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="10"/>
       <c r="C23" s="12"/>
@@ -982,7 +1011,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="10"/>
       <c r="C24" s="12"/>
@@ -991,33 +1020,33 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+    <row r="25" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="2"/>
@@ -1026,8 +1055,9 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1330,12 +1360,20 @@
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>